<commit_message>
starting to call sample metadata update service
</commit_message>
<xml_diff>
--- a/test/fixtures/files/metadata/valid.xlsx
+++ b/test/fixtures/files/metadata/valid.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">sample_id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">sample_name</t>
   </si>
   <si>
     <t xml:space="preserve">metadatafield1</t>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">metadatafield3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 1 Sample 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 1 Sample 2</t>
   </si>
 </sst>
 </file>
@@ -46,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,8 +112,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,66 +141,58 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>40</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
starting to remove data types when save sample & pipeline metadata
</commit_message>
<xml_diff>
--- a/test/fixtures/files/metadata/valid.xlsx
+++ b/test/fixtures/files/metadata/valid.xlsx
@@ -141,10 +141,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
testing uppercase metadata values
</commit_message>
<xml_diff>
--- a/test/fixtures/files/metadata/valid.xlsx
+++ b/test/fixtures/files/metadata/valid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -37,28 +37,38 @@
     <t xml:space="preserve">metadatafield4</t>
   </si>
   <si>
+    <t xml:space="preserve">metadatafield5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project 1 Sample 1</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
   </si>
   <si>
+    <t xml:space="preserve">A Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project 1 Sample 2</t>
   </si>
   <si>
     <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,11 +89,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,15 +142,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,13 +171,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
   </cols>
@@ -190,38 +195,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">DATE(24,1,4)</f>
         <v>45295</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">DATE(24,12,31)</f>
         <v>45657</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Metadata: Update values to strings (#808)
* starting to remove data types when save sample & pipeline metadata

* removing data types from seed metadata

* starting to add a db migration to lowercase the sample metadata

* adding a graphql test

* testing datatypes

* undoing changes to seeds.rb as it uses the metadata update service

* testing uppercase metadata values

* reverting downcasing metadata values

* removing comments

* updating the metadata update service to strip whitespace for keys and values

* adding and updating tests

* fixing migration query
</commit_message>
<xml_diff>
--- a/test/fixtures/files/metadata/valid.xlsx
+++ b/test/fixtures/files/metadata/valid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -34,18 +34,39 @@
     <t xml:space="preserve">metadatafield3</t>
   </si>
   <si>
+    <t xml:space="preserve">metadatafield4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metadatafield5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project 1 Sample 1</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project 1 Sample 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -112,12 +133,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -138,13 +171,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -159,33 +195,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>30</v>
+      <c r="C2" s="2" t="n">
+        <f aca="false">DATE(24,1,4)</f>
+        <v>45295</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>35</v>
+      <c r="C3" s="2" t="n">
+        <f aca="false">DATE(24,12,31)</f>
+        <v>45657</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>